<commit_message>
Amaro Romão - 11/06/2018
</commit_message>
<xml_diff>
--- a/Hydra.Such.Portal/Hydra.Such.Portal/wwwroot/Upload/FH_PrecoVendaRecursos_Template.xlsx
+++ b/Hydra.Such.Portal/Hydra.Such.Portal/wwwroot/Upload/FH_PrecoVendaRecursos_Template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ARomao\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_GITHUB\Hydra.Such.Portal\Hydra.Such.Portal\Hydra.Such.Portal\wwwroot\Upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FB87AE68-029E-48A5-8FB6-6457443762A4}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1982C295-78CC-49FA-A4E6-E411B14D7302}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7800" xr2:uid="{D71C0A71-CDA0-46D8-AC1E-52B57A94F319}"/>
   </bookViews>

</xml_diff>